<commit_message>
Update 1: Fixed test cases
</commit_message>
<xml_diff>
--- a/Class12/Class12Capstone/Test Cases/API Specific Tests and Results/TCAPI.xlsx
+++ b/Class12/Class12Capstone/Test Cases/API Specific Tests and Results/TCAPI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10785" yWindow="-15" windowWidth="5430" windowHeight="18120"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10800" windowHeight="18195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>AC1: Able to add new veteranian</t>
   </si>
@@ -24,21 +24,6 @@
     <t xml:space="preserve"> Assumptions:</t>
   </si>
   <si>
-    <t>Google chrome browser is installed and opened on windows surface</t>
-  </si>
-  <si>
-    <t>The website is connected to the server with internet</t>
-  </si>
-  <si>
-    <t>User is able to login successfully as vet_admin</t>
-  </si>
-  <si>
-    <t>User knows how to navigate the website and add new veteranian</t>
-  </si>
-  <si>
-    <t>Bugmagnet and JSON view are installed in the browser</t>
-  </si>
-  <si>
     <t>Valid Name input is at least 2 characters and less than 31 characters long</t>
   </si>
   <si>
@@ -51,9 +36,6 @@
     <t>Test Steps</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Data </t>
-  </si>
-  <si>
     <t>Expected Result</t>
   </si>
   <si>
@@ -66,35 +48,20 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>AC1TC10: Add new Veterinarian with invalid first and valid last name, and Specialty Type</t>
-  </si>
-  <si>
-    <t>1. User enters valid username and password to login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username: vet_admin password: </t>
-  </si>
-  <si>
-    <t>Logs in as vet_admin and displays homepage</t>
-  </si>
-  <si>
     <t>postman</t>
   </si>
   <si>
-    <t>2. Click on Veterinarian drop down menu</t>
-  </si>
-  <si>
-    <t>Displays ALL and ADD NEW buttons</t>
-  </si>
-  <si>
-    <t>3. Click on ADD NEW button on the Veterinarian drop down menu</t>
-  </si>
-  <si>
-    <t>Displays New Veterinarian form with First Name, Last Name, and Type input box. Back and Save Vet buttons.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4. Enter </t>
+    <t>POSTMAN is installed</t>
+  </si>
+  <si>
+    <t>Authentication data are current</t>
+  </si>
+  <si>
+    <t>API Body data and its format are provided</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AC1TC10: Add new Veterinarian with </t>
     </r>
     <r>
       <rPr>
@@ -104,15 +71,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>invalid First Name</t>
-    </r>
-  </si>
-  <si>
-    <t>Displays error message: First name must be at least 2 characters long</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. Enter </t>
+      <t xml:space="preserve">invalid first </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -122,51 +100,118 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>valid Last Name</t>
-    </r>
-  </si>
-  <si>
-    <t>Displays no error messages</t>
-  </si>
-  <si>
-    <t>6. Click on Type drop down list</t>
-  </si>
-  <si>
-    <t>Displays a list of Veterinarian specialties</t>
-  </si>
-  <si>
-    <t>7. Click on random specialty type</t>
-  </si>
-  <si>
-    <t>Displays the chosen specialty in the Type box</t>
-  </si>
-  <si>
-    <t>8. Click on Save Vet button</t>
-  </si>
-  <si>
-    <t>Displays error message: Error in 1 or more fields. Will not save the new Veterinarian info</t>
-  </si>
-  <si>
-    <t>AC1TC11: Add new Veterinarian with valid first and invalid last name, and Specialty Type</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4. Enter </t>
+      <t>valid last name</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF37E93B"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>valid First Name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. Enter </t>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Specialty Type </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>through API</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Create a new Request for POST with https://clinic.doveryai-no-proveryai.com/petclinic/api/vets/</t>
+  </si>
+  <si>
+    <t>2. Click on Authorization tab</t>
+  </si>
+  <si>
+    <t>3. Select Basic Auth on Type drop down list</t>
+  </si>
+  <si>
+    <t>4. Enter Username</t>
+  </si>
+  <si>
+    <t>vet_admin</t>
+  </si>
+  <si>
+    <t>5. Enter Password</t>
+  </si>
+  <si>
+    <t>6. Click on Body tab</t>
+  </si>
+  <si>
+    <t>Displays Body input area</t>
+  </si>
+  <si>
+    <t>7. Copy paste the Body data in JSON format from the text file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC1TC10and11body.txt </t>
+  </si>
+  <si>
+    <t>8. Select JSON on Body type</t>
+  </si>
+  <si>
+    <t>1. a                                                2. z                                                3. X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. De Cow                                  2. Just Cow                                3. Cow Pow </t>
+  </si>
+  <si>
+    <t>10. Change specialties "id"</t>
+  </si>
+  <si>
+    <t>12. Cick Send</t>
+  </si>
+  <si>
+    <t>Status: 400 Bad Request             Displays "Could not execute statement" on the Response Body tab</t>
+  </si>
+  <si>
+    <t>1. Moo                                         2. Cowdepow                           3. Austin</t>
+  </si>
+  <si>
+    <t>15. Change specialties "id"</t>
+  </si>
+  <si>
+    <t>16. Click Send</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AC1TC11: Add new Veterinarian with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valid first</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
     </r>
     <r>
       <rPr>
@@ -176,24 +221,86 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>invalid Last Name</t>
-    </r>
-  </si>
-  <si>
-    <t>Displays error message: Last name must be at least 2 characters long</t>
-  </si>
-  <si>
-    <t>Displays a list of veteranians specialties</t>
-  </si>
-  <si>
-    <t>Displays error message: Error in 1 or more fields. Will not save the new veteranian info</t>
+      <t>invalid last name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Specialty Type </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>through API</t>
+    </r>
+  </si>
+  <si>
+    <t>1.qwertyuiopasdfghjklzxcvbnmqwert                                   2.mnbvcxzlkjhgfdsapoiuytrewqmnbvc                                3.qazwsxedcrfvtgbyhnujmikolpqazws</t>
+  </si>
+  <si>
+    <t>Test Data  / Script</t>
+  </si>
+  <si>
+    <t>Input less than 2 characters for First Name</t>
+  </si>
+  <si>
+    <t>9. Insert firstName data between the quotes</t>
+  </si>
+  <si>
+    <t>10. Insert lastName data between the qoutes</t>
+  </si>
+  <si>
+    <t>11. Change specialties "id"</t>
+  </si>
+  <si>
+    <t>Input more than 30 characters for First Name</t>
+  </si>
+  <si>
+    <t>13. Insert firstName data between the quotes</t>
+  </si>
+  <si>
+    <t>1.qwertyuiopasdfghjklzxcvbnmqwert                                  2.mnbvcxzlkjhgfdsapoiuytrewqmnbvc                                3.qazwsxedcrfvtgbyhnujmikolpqazws</t>
+  </si>
+  <si>
+    <t>14. Insert lastName data between the qoutes</t>
+  </si>
+  <si>
+    <t>9. Insert firstName data between the qoutes</t>
+  </si>
+  <si>
+    <t>Input more than 30 characters for Last Name</t>
+  </si>
+  <si>
+    <t>13. Insert firstName data between the qoutes</t>
+  </si>
+  <si>
+    <t>Input less than 2 characters for Last Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,15 +351,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF37E93B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,8 +377,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,39 +420,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="medium">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="medium">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="medium">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="medium">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -370,17 +448,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -703,281 +778,463 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A10" t="s">
+      <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>22</v>
-      </c>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="60.75" thickBot="1">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="45.75" thickBot="1">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1">
       <c r="A15" s="3"/>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="7" t="s">
-        <v>26</v>
+      <c r="D15" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+    <row r="16" spans="1:7" ht="45.75" thickBot="1">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="8" t="s">
-        <v>28</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="8"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A17" s="6"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>32</v>
-      </c>
+    <row r="18" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A19" s="6"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A20" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="60.75" thickBot="1">
+      <c r="A21" s="3"/>
       <c r="B21" s="6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="60.75" thickBot="1">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:7" ht="105.75" thickBot="1">
+      <c r="A22" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:7" ht="45.75" thickBot="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="30.75" thickBot="1">
+      <c r="B23" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1">
       <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" ht="30.75" thickBot="1">
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="4">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="60.75" thickBot="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="105.75" thickBot="1">
+      <c r="A35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+      <c r="C35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" ht="60.75" thickBot="1">
+      <c r="A37" s="3"/>
+      <c r="B37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A39" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
+      <c r="C40" s="4">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" ht="60.75" thickBot="1">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>